<commit_message>
Add cumulative daily penalty tracking and display total penalties per player
Update penalty tracking system to include cumulative daily penalty sums and display each player's total accumulated penalties.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: dd5db95a-98b7-43c9-ad5e-b8ec16e69a70
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ec40b5de-34a1-4de4-ab37-5df875677ee8/dd5db95a-98b7-43c9-ad5e-b8ec16e69a70/cP4HhpS
</commit_message>
<xml_diff>
--- a/Strafenerfassung_ASV_Natz.xlsx
+++ b/Strafenerfassung_ASV_Natz.xlsx
@@ -417,289 +417,6 @@
 </table>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add user login and role-based access controls for different user types
Implement a login system with distinct roles (player and treasurer) using access codes, session management, and decorators to enforce permissions on various application routes. Adds a new login page and modifies existing navigation and route protection.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: dd5db95a-98b7-43c9-ad5e-b8ec16e69a70
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ec40b5de-34a1-4de4-ab37-5df875677ee8/dd5db95a-98b7-43c9-ad5e-b8ec16e69a70/GObvBoR
</commit_message>
<xml_diff>
--- a/Strafenerfassung_ASV_Natz.xlsx
+++ b/Strafenerfassung_ASV_Natz.xlsx
@@ -417,6 +417,289 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Initial import from Replit
</commit_message>
<xml_diff>
--- a/Strafenerfassung_ASV_Natz.xlsx
+++ b/Strafenerfassung_ASV_Natz.xlsx
@@ -417,289 +417,6 @@
 </table>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Improve system stability and fix connection issues
Fix connection refused error when loading the application on Streamlit by ensuring proper server configuration and port handling.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0dc3cae5-e05b-4536-9323-52f33c2c309b
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ec40b5de-34a1-4de4-ab37-5df875677ee8/0dc3cae5-e05b-4536-9323-52f33c2c309b/MIg1Lj0
</commit_message>
<xml_diff>
--- a/Strafenerfassung_ASV_Natz.xlsx
+++ b/Strafenerfassung_ASV_Natz.xlsx
@@ -417,6 +417,289 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>